<commit_message>
Changes to be committed: 	modified:   Results.xlsx
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,48 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alireza/Desktop/Sharif 1401-1/VRPTWM/MPMAVRPMain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B5F433-F538-F043-87C7-DF7302D5FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86FBA43-0C1C-9E45-A8AF-4F36BA58A06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{1F5CCFC7-61F6-154E-BDAB-8D5A3730E25A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{1F5CCFC7-61F6-154E-BDAB-8D5A3730E25A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Memetic A" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Memetic A'!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Memetic A'!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Memetic A'!$K$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Memetic A'!$K$2:$K$21</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Memetic A'!$M$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Memetic A'!$M$2:$M$21</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'Memetic A'!$O$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'Memetic A'!$O$2:$O$21</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Memetic A'!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Memetic A'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Memetic A'!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Memetic A'!$E$2:$E$21</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Memetic A'!$G$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Memetic A'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Memetic A'!$I$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Memetic A'!$I$2:$I$21</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">'Memetic A'!$A$1</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">'Memetic A'!$A$2:$A$21</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">'Memetic A'!$C$1</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">'Memetic A'!$C$2:$C$21</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">'Memetic A'!$E$1</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">'Memetic A'!$E$2:$E$21</definedName>
-    <definedName name="_xlchart.v2.22" hidden="1">'Memetic A'!$G$1</definedName>
-    <definedName name="_xlchart.v2.23" hidden="1">'Memetic A'!$G$2:$G$21</definedName>
-    <definedName name="_xlchart.v2.24" hidden="1">'Memetic A'!$I$1</definedName>
-    <definedName name="_xlchart.v2.25" hidden="1">'Memetic A'!$I$2:$I$21</definedName>
-    <definedName name="_xlchart.v2.26" hidden="1">'Memetic A'!$K$1</definedName>
-    <definedName name="_xlchart.v2.27" hidden="1">'Memetic A'!$K$2:$K$21</definedName>
-    <definedName name="_xlchart.v2.28" hidden="1">'Memetic A'!$M$1</definedName>
-    <definedName name="_xlchart.v2.29" hidden="1">'Memetic A'!$M$2:$M$21</definedName>
-    <definedName name="_xlchart.v2.30" hidden="1">'Memetic A'!$O$1</definedName>
-    <definedName name="_xlchart.v2.31" hidden="1">'Memetic A'!$O$2:$O$21</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -346,26 +312,32 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -374,12 +346,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1676,9 +1642,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1735,9 +1701,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1777,9 +1743,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1810,7 +1776,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3106,9 +3075,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3165,9 +3134,9 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3212,9 +3181,9 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3246,7 +3215,10 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4700,1710 +4672,1774 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E23C40E-058B-C443-80DE-840D89B0A043}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView topLeftCell="G25" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I34" sqref="I34:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="4">
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2">
         <v>5413.6016312043002</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="E3" s="8"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2">
         <v>30062.555423941802</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="4">
+      <c r="I3" s="8"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2">
         <v>105386.123930243</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="11" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="2">
         <v>13</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="4">
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="A5" s="8"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2">
         <v>10970.4325464169</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="E5" s="8"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2">
         <v>263794.24730262201</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="4">
+      <c r="I5" s="8"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2">
         <v>764003.98859426298</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2">
         <v>14</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="11" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
         <v>15570.7068366069</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="2">
         <v>116580.97639304399</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="4">
+      <c r="I7" s="8"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2">
         <v>649960.38991162204</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2">
         <v>15</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="11" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2">
         <v>22310.9264365778</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="E9" s="8"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2">
         <v>192722.638912772</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="4">
+      <c r="I9" s="8"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="2">
         <v>418610.34283880203</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2">
         <v>14</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2">
         <v>7902.3845187549596</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="E11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="2">
         <v>36089.543625275903</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="4">
+      <c r="I11" s="8"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="2">
         <v>140757.42870126999</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
         <v>6</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2">
         <v>12</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="11" t="s">
+      <c r="I12" s="8"/>
+      <c r="J12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="4">
+      <c r="K12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="A13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
         <v>61613.5931986367</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="E13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="2">
         <v>282901.72174095601</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="I13" s="8"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="2">
         <v>435528.182622661</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="11" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2">
         <v>7</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="8"/>
+      <c r="F14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="2">
         <v>13</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="11" t="s">
+      <c r="I14" s="8"/>
+      <c r="J14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="A15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
         <v>14923.0743999346</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="E15" s="8"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="2">
         <v>111785.467592778</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="4">
+      <c r="I15" s="8"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="2">
         <v>392624.78995355702</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2">
         <v>6</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="8"/>
+      <c r="F16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="G16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="11" t="s">
+      <c r="I16" s="8"/>
+      <c r="J16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="A17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
         <v>37355.080396887999</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="E17" s="8"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="4" t="s">
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
         <v>5</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="2">
         <v>15</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="4">
+      <c r="K18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
         <v>6715.7352643863596</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="E19" s="8"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="2">
         <v>33376.521012814497</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="4">
+      <c r="I19" s="8"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="2">
         <v>93603.275863004907</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
         <v>6</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="11" t="s">
+      <c r="E20" s="8"/>
+      <c r="F20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="4">
+      <c r="G20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="2">
         <v>14</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="11" t="s">
+      <c r="I20" s="8"/>
+      <c r="J20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="4">
+      <c r="K20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="A21" s="8"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2">
         <v>20669.003534371099</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="4">
+      <c r="E21" s="8"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="2">
         <v>224354.60833692201</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" s="4">
+      <c r="I21" s="8"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="2">
         <v>764003.98859426298</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="11" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2">
         <v>6</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="11" t="s">
+      <c r="E22" s="8"/>
+      <c r="F22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="4">
+      <c r="G22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="2">
         <v>14</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="11" t="s">
+      <c r="I22" s="8"/>
+      <c r="J22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="4">
+      <c r="K22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="A23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2">
         <v>20669.003534371099</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="4">
+      <c r="E23" s="8"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="2">
         <v>82186.568920721693</v>
       </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L23" s="4">
+      <c r="I23" s="8"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="2">
         <v>649960.38991162204</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="2">
         <v>6</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="8"/>
+      <c r="F24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="4">
+      <c r="G24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="2">
         <v>14</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="11" t="s">
+      <c r="I24" s="8"/>
+      <c r="J24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="4">
+      <c r="K24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4">
+      <c r="A25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2">
         <v>20669.003534371099</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="4">
+      <c r="E25" s="8"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="2">
         <v>185546.483836706</v>
       </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="4">
+      <c r="I25" s="8"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" s="2">
         <v>418610.34283880203</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="4">
+      <c r="C26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2">
         <v>5</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="G26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2">
         <v>11</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="4">
+      <c r="K26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="4">
+      <c r="A27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2">
         <v>5771.9470575947798</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="E27" s="8"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="2">
         <v>29290.820952567199</v>
       </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L27" s="4">
+      <c r="I27" s="8"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="2">
         <v>106168.06374706</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="11" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="4">
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2">
         <v>6</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="8"/>
+      <c r="F28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="4">
+      <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="2">
         <v>12</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="11" t="s">
+      <c r="I28" s="8"/>
+      <c r="J28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="4">
+      <c r="K28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="4">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="2">
         <v>30831.2775727306</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="4">
+      <c r="E29" s="8"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2">
         <v>190232.10299182701</v>
       </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L29" s="4">
+      <c r="I29" s="8"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="2">
         <v>435528.182622661</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="4">
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2">
         <v>8</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="11" t="s">
+      <c r="E30" s="8"/>
+      <c r="F30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="4">
+      <c r="G30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="2">
         <v>12</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="11" t="s">
+      <c r="I30" s="8"/>
+      <c r="J30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="4">
+      <c r="K30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="4">
+      <c r="A31" s="8"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="2">
         <v>25751.477158434001</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="E31" s="8"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="2">
         <v>126095.92953535001</v>
       </c>
-      <c r="I31" s="2"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L31" s="4">
+      <c r="I31" s="8"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="2">
         <v>392624.78995355702</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="11" t="s">
+      <c r="E32" s="8"/>
+      <c r="F32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="G32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="2">
         <v>13</v>
       </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="11" t="s">
+      <c r="I32" s="8"/>
+      <c r="J32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="4" t="s">
+      <c r="K32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="A33" s="8"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="E33" s="8"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="2">
         <v>96399.026026126099</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L33" s="4" t="s">
+      <c r="I33" s="8"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="4">
+      <c r="C34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="2">
         <v>5</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="4">
+      <c r="G34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="2">
         <v>16</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J34" s="11" t="s">
+      <c r="J34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="4">
+      <c r="K34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="4">
+      <c r="A35" s="8"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2">
         <v>5657.1879104616701</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="4">
+      <c r="E35" s="8"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="2">
         <v>41748.502787220197</v>
       </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L35" s="4">
+      <c r="I35" s="8"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35" s="2">
         <v>140808.2221741</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="11" t="s">
+      <c r="A36" s="8"/>
+      <c r="B36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="4">
+      <c r="C36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2">
         <v>6</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="11" t="s">
+      <c r="E36" s="8"/>
+      <c r="F36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="4">
+      <c r="G36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="2">
         <v>13</v>
       </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="11" t="s">
+      <c r="I36" s="8"/>
+      <c r="J36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="4">
+      <c r="K36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="4">
+      <c r="A37" s="8"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2">
         <v>13794.7743908625</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="4">
+      <c r="E37" s="8"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="2">
         <v>378811.63873626199</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L37" s="4">
+      <c r="I37" s="8"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37" s="2">
         <v>421188.391849601</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="11" t="s">
+      <c r="A38" s="8"/>
+      <c r="B38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="4">
+      <c r="C38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="2">
         <v>6</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="11" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="4">
+      <c r="G38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="2">
         <v>13</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="11" t="s">
+      <c r="I38" s="8"/>
+      <c r="J38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="4">
+      <c r="K38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="4">
+      <c r="A39" s="8"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="2">
         <v>34174.4884901123</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="4">
+      <c r="E39" s="8"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="2">
         <v>172809.47004046899</v>
       </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L39" s="4">
+      <c r="I39" s="8"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39" s="2">
         <v>454336.63828143501</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="11" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="4">
+      <c r="C40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="2">
         <v>6</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="11" t="s">
+      <c r="E40" s="8"/>
+      <c r="F40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="4">
+      <c r="G40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="2">
         <v>12</v>
       </c>
-      <c r="I40" s="2"/>
-      <c r="J40" s="11" t="s">
+      <c r="I40" s="8"/>
+      <c r="J40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K40" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="4">
+      <c r="K40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="4">
+      <c r="A41" s="8"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2">
         <v>13794.7743908625</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="E41" s="8"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="2">
         <v>334983.12523165502</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L41" s="4">
+      <c r="I41" s="8"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41" s="2">
         <v>1147450.09751855</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="4">
+      <c r="C42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="2">
         <v>4</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="4">
+      <c r="G42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="2">
         <v>15</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I42" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="J42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="4">
+      <c r="K42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="2">
         <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="4">
+      <c r="A43" s="8"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="2">
         <v>5435.4413065872895</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="4">
+      <c r="E43" s="8"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="2">
         <v>29201.913254575898</v>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L43" s="4">
+      <c r="I43" s="8"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43" s="2">
         <v>100373.405681273</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="11" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="4">
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="2">
         <v>6</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="11" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="4">
+      <c r="G44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="2">
         <v>13</v>
       </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="11" t="s">
+      <c r="I44" s="8"/>
+      <c r="J44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="4">
+      <c r="K44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="4">
+      <c r="A45" s="8"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="2">
         <v>15340.823124508899</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" s="4">
+      <c r="E45" s="8"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H45" s="2">
         <v>263794.24730262201</v>
       </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L45" s="4">
+      <c r="I45" s="8"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L45" s="2">
         <v>1925460.12087797</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="11" t="s">
+      <c r="A46" s="8"/>
+      <c r="B46" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="4">
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="2">
         <v>6</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="11" t="s">
+      <c r="E46" s="8"/>
+      <c r="F46" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="4">
+      <c r="G46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="2">
         <v>14</v>
       </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="11" t="s">
+      <c r="I46" s="8"/>
+      <c r="J46" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="4">
+      <c r="K46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="4">
+      <c r="A47" s="8"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="2">
         <v>15340.823124508899</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="E47" s="8"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="2">
         <v>116580.97639304399</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L47" s="4">
+      <c r="I47" s="8"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L47" s="2">
         <v>382714.83845500898</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="11" t="s">
+      <c r="A48" s="8"/>
+      <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D48" s="4" t="s">
+      <c r="C48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="11" t="s">
+      <c r="E48" s="8"/>
+      <c r="F48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="4">
+      <c r="G48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="2">
         <v>15</v>
       </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="11" t="s">
+      <c r="I48" s="8"/>
+      <c r="J48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="4">
+      <c r="K48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="4" t="s">
+      <c r="A49" s="8"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H49" s="4">
+      <c r="E49" s="8"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="2">
         <v>192722.638912772</v>
       </c>
-      <c r="I49" s="2"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L49" s="4">
+      <c r="I49" s="8"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49" s="2">
         <v>710946.01795733499</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="4">
+      <c r="C50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="2">
         <v>5</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="4">
+      <c r="G50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="2">
         <v>14</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J50" s="11" t="s">
+      <c r="J50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="4">
+      <c r="K50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="4">
+      <c r="A51" s="8"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="2">
         <v>6381.4447100972702</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" s="4">
+      <c r="E51" s="8"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H51" s="2">
         <v>47181.225943359401</v>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L51" s="4">
+      <c r="I51" s="8"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51" s="2">
         <v>103943.69706914001</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-      <c r="B52" s="11" t="s">
+      <c r="A52" s="8"/>
+      <c r="B52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52" s="4">
+      <c r="C52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" s="2">
         <v>5</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="11" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="4">
+      <c r="G52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="2">
         <v>13</v>
       </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="11" t="s">
+      <c r="I52" s="8"/>
+      <c r="J52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K52" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="4">
+      <c r="K52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="4">
+      <c r="A53" s="8"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="2">
         <v>32496.5454953802</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="4">
+      <c r="E53" s="8"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="2">
         <v>244663.248959444</v>
       </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L53" s="4">
+      <c r="I53" s="8"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53" s="2">
         <v>764003.98859426298</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
-      <c r="B54" s="11" t="s">
+      <c r="A54" s="8"/>
+      <c r="B54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="4">
+      <c r="C54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="2">
         <v>4</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="11" t="s">
+      <c r="E54" s="8"/>
+      <c r="F54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" s="4">
+      <c r="G54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="2">
         <v>13</v>
       </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="11" t="s">
+      <c r="I54" s="8"/>
+      <c r="J54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L54" s="4">
+      <c r="K54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55" s="4">
+      <c r="A55" s="8"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="2">
         <v>35451.076589153199</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="4">
+      <c r="E55" s="8"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="2">
         <v>261541.88178613299</v>
       </c>
-      <c r="I55" s="2"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L55" s="4">
+      <c r="I55" s="8"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="2">
         <v>649960.38991162204</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
-      <c r="B56" s="11" t="s">
+      <c r="A56" s="8"/>
+      <c r="B56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="4">
+      <c r="C56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="2">
         <v>4</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="11" t="s">
+      <c r="E56" s="8"/>
+      <c r="F56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" s="4" t="s">
+      <c r="G56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="11" t="s">
+      <c r="I56" s="8"/>
+      <c r="J56" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="4">
+      <c r="K56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="7">
+      <c r="A57" s="9"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="4">
         <v>35451.076589153199</v>
       </c>
-      <c r="E57" s="5"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" s="7" t="s">
+      <c r="E57" s="9"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I57" s="5"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L57" s="7">
+      <c r="I57" s="9"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57" s="4">
         <v>418610.34283880203</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="J42:J43"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:E9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="E10:E17"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="E26:E33"/>
+    <mergeCell ref="E34:E41"/>
+    <mergeCell ref="E42:E49"/>
+    <mergeCell ref="E50:E57"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I2:I9"/>
+    <mergeCell ref="I10:I17"/>
+    <mergeCell ref="I18:I25"/>
+    <mergeCell ref="I26:I33"/>
+    <mergeCell ref="I34:I41"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I42:I49"/>
+    <mergeCell ref="I50:I57"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F28:F29"/>
     <mergeCell ref="J26:J27"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="J30:J31"/>
@@ -6428,80 +6464,16 @@
     <mergeCell ref="F52:F53"/>
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="I42:I49"/>
-    <mergeCell ref="I50:I57"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="I2:I9"/>
-    <mergeCell ref="I10:I17"/>
-    <mergeCell ref="I18:I25"/>
-    <mergeCell ref="I26:I33"/>
-    <mergeCell ref="I34:I41"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="E10:E17"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="E26:E33"/>
-    <mergeCell ref="E34:E41"/>
-    <mergeCell ref="E42:E49"/>
-    <mergeCell ref="E50:E57"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:E9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="J48:J49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6512,8 +6484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD72069-436E-D64A-A693-D25E065E2834}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="Q52" sqref="Q52"/>
+    <sheetView topLeftCell="A12" zoomScale="83" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>